<commit_message>
Updated test case for commit ID 3
Check note section and enhancement of a testcase
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yesha\Desktop\Test\QualityAssurance\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yesha\Desktop\QA\QualityAssurance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>SR#</t>
   </si>
@@ -53,18 +53,47 @@
     <t>Enter Valid userID &amp; Password</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Go To http://demo.guru99.com/
+    <t>userID
+Password</t>
+  </si>
+  <si>
+    <t>Login Successfully</t>
+  </si>
+  <si>
+    <t>1. Go To http://demo.guru99.com/
 2.  Enter Valid userID
 3. Enter valid password
 4. Click Login
-</t>
-  </si>
-  <si>
-    <t>userID
-Password</t>
-  </si>
-  <si>
-    <t>Login Successfully</t>
+5. Verify the output</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Task for Commit 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: The code to setup and launch WebDriver (Firefox) should be improved to include Location   Firefox.exe    and a Firefox Profile must be created.
+The amount of time the driver should wait when searching for a GUI element should be specified
+The code to setup and launch Firefox should be created as a separate method.
+All script initialization parameters like Location of Firefox , Base URL, User Name , Password etc should be stored in separate file say Util.java.  This helps in easy maintenance of script</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -108,12 +137,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -437,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,9 +476,10 @@
     <col min="4" max="4" width="37.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="63.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,25 +498,31 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ID: 3 #TestCase Update : Refer note section of test case
1.The code to setup and launch WebDriver (Firefox) should be improved to
include Location   Firefox.exe    and a Firefox Profile must be created.
2.The amount of time the driver should wait when searching for a GUI
element should be specified
The code to setup and launch Firefox should be created as a separate
method.
3.All script initialization parameters like Location of Firefox , Base
URL, User Name , Password etc should be stored in separate file say
Util.java.  This helps in easy maintenance of script
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -89,10 +89,94 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: The code to setup and launch WebDriver (Firefox) should be improved to include Location   Firefox.exe    and a Firefox Profile must be created.
-The amount of time the driver should wait when searching for a GUI element should be specified
-The code to setup and launch Firefox should be created as a separate method.
-All script initialization parameters like Location of Firefox , Base URL, User Name , Password etc should be stored in separate file say Util.java.  This helps in easy maintenance of script</t>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. The code to setup and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">launch WebDriver (Firefox) should be improved to include Location   Firefox.exe    and a Firefox Profile must be created.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2. The amount of time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the driver should wait when searching for a GUI element should be specified
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">3.The code to setup and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">launch Firefox should be created as a separate method.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4. All script initialization parameters li</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ke Location of Firefox , Base URL, User Name , Password etc should be stored in separate file say Util.java.  This helps in easy maintenance of script</t>
     </r>
   </si>
 </sst>

</xml_diff>

<commit_message>
Test case updated to achieve ID 4
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>SR#</t>
   </si>
@@ -178,6 +178,137 @@
       </rPr>
       <t>ke Location of Firefox , Base URL, User Name , Password etc should be stored in separate file say Util.java.  This helps in easy maintenance of script</t>
     </r>
+  </si>
+  <si>
+    <t>ss1.1</t>
+  </si>
+  <si>
+    <t>PARAMETRIZATION SCRIPT</t>
+  </si>
+  <si>
+    <t>SS2</t>
+  </si>
+  <si>
+    <t>Enter Invalid user id &amp; valid Password</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>valid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> user id &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>invalid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Password</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>invalid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> user id &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>invalid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Password</t>
+    </r>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <t>userID = valid
+Password = valid</t>
+  </si>
+  <si>
+    <t>userID = valid
+Password = invalid</t>
+  </si>
+  <si>
+    <t>userID =invalid
+Password = valid</t>
+  </si>
+  <si>
+    <t>userID =invalid
+Password = invalid</t>
+  </si>
+  <si>
+    <t>A pop-up "User or Password is not valid" - Shown</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -221,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -232,6 +363,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +746,91 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:G3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>